<commit_message>
Updated Pattern FD file
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.TestDataGenerator.Functors/FD/Manual/FD Rules Control File.xlsx
+++ b/src/ESFA.DC.ILR.TestDataGenerator.Functors/FD/Manual/FD Rules Control File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAwaghade\OneDrive - Department for Education\Documents\ESFA\FD Rules Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{2E12C40A-DB92-427E-9175-BC7CC62A423E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{0C5731F5-7001-40E0-9EC5-67184F5CB318}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{2E12C40A-DB92-427E-9175-BC7CC62A423E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{6BBCA4B5-33FF-40C2-AF43-E06CBD84461A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FD Rules" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="690">
   <si>
     <t>Sr. No</t>
   </si>
@@ -2094,6 +2094,12 @@
   </si>
   <si>
     <t>Error Type</t>
+  </si>
+  <si>
+    <t>P229AgreeID</t>
+  </si>
+  <si>
+    <t>FD_AgreeId_AP</t>
   </si>
 </sst>
 </file>
@@ -2236,7 +2242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2416,18 +2422,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2604,12 +2598,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2965,16 +2957,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E229"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
@@ -3577,19 +3568,19 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3695,7 +3686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3712,7 +3703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3729,7 +3720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3746,7 +3737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3763,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3780,7 +3771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3797,7 +3788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3814,449 +3805,449 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="E50" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="E51" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="E52" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="E53" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="E54" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>54</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="E55" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="E56" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="E57" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="E58" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="E59" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="E60" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="E61" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="E62" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="E63" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="E64" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="E65" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="E66" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="E67" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="E68" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="E69" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>69</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="E70" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>70</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="E71" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>71</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="E72" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>72</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="E73" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>73</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="E74" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
         <v>74</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4273,7 +4264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -4290,7 +4281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4307,7 +4298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4324,7 +4315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4341,7 +4332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -4358,7 +4349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -4375,7 +4366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -4392,41 +4383,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
         <v>83</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E84" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="E84" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
         <v>84</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E85" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E85" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -4443,7 +4434,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -4460,41 +4451,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
         <v>87</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E88" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="E88" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
         <v>88</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E89" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E89" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -4511,7 +4502,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -4528,7 +4519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -4545,41 +4536,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
         <v>92</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E93" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="E93" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
         <v>93</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E94" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E94" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -4596,7 +4587,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -4613,7 +4604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -4630,41 +4621,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
         <v>97</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="E98" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
         <v>98</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E99" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E99" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -4681,7 +4672,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -4698,7 +4689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -4715,41 +4706,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
         <v>102</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E103" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="E103" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
         <v>103</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E104" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E104" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -4766,7 +4757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -4783,41 +4774,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
         <v>106</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E107" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+      <c r="E107" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
         <v>107</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E108" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E108" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -4834,41 +4825,41 @@
         <v>685</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
         <v>109</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E110" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="E110" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
         <v>110</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E111" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E111" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -4885,7 +4876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -4902,7 +4893,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -4919,7 +4910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -4936,41 +4927,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
         <v>115</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="E116" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="E116" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
         <v>116</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="E117" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E117" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -4987,7 +4978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -5004,7 +4995,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -5021,7 +5012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -5038,7 +5029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -5055,7 +5046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -5072,7 +5063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -5089,7 +5080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -5106,7 +5097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -5123,7 +5114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -5140,364 +5131,364 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
         <v>127</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="E128" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
+      <c r="E128" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
         <v>128</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C129" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="E129" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="E129" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
         <v>129</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D130" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="E130" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="E130" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
         <v>130</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E131" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="E131" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
         <v>131</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E132" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+      <c r="E132" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
         <v>132</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E133" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+      <c r="E133" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
         <v>133</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E134" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+      <c r="E134" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
         <v>134</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E135" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="E135" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
         <v>135</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E136" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
+      <c r="E136" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
         <v>136</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C137" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E137" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="E137" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
         <v>137</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="E138" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+      <c r="E138" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
         <v>138</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="E139" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
+      <c r="E139" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
         <v>139</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E140" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
+      <c r="E140" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
         <v>140</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="E141" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="4">
+      <c r="E141" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
         <v>141</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="E142" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="E142" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
         <v>142</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="E143" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="4">
+      <c r="E143" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
         <v>143</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E144" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="4">
+      <c r="E144" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
         <v>144</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C145" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="D145" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="E145" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="E145" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
         <v>145</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D146" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E146" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="4">
+      <c r="E146" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
         <v>146</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C147" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D147" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E147" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="4">
+      <c r="E147" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
         <v>147</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D148" s="4" t="s">
+      <c r="D148" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="E148" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E148" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -5514,7 +5505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -5531,7 +5522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -5548,7 +5539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -5565,7 +5556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -5582,7 +5573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -5599,7 +5590,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -5616,7 +5607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -5633,41 +5624,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="4">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
         <v>156</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C157" s="4" t="s">
+      <c r="C157" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="D157" s="4" t="s">
+      <c r="D157" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="E157" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="4">
+      <c r="E157" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
         <v>157</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C158" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="D158" s="4" t="s">
+      <c r="D158" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="E158" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E158" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -5684,7 +5675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -5701,7 +5692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -5718,58 +5709,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="4">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
         <v>161</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C162" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="D162" s="4" t="s">
+      <c r="D162" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="E162" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="4">
+      <c r="E162" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
         <v>162</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="D163" s="4" t="s">
+      <c r="D163" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="E163" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="4">
+      <c r="E163" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
         <v>163</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D164" s="4" t="s">
+      <c r="D164" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="E164" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E164" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -5786,7 +5777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -5803,7 +5794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -5820,7 +5811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -5837,7 +5828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -5854,58 +5845,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="4">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
         <v>169</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B170" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="D170" s="4" t="s">
+      <c r="D170" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="E170" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="4">
+      <c r="E170" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
         <v>170</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B171" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="C171" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D171" s="4" t="s">
+      <c r="D171" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="E171" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="4">
+      <c r="E171" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
         <v>171</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B172" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="C172" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="D172" s="4" t="s">
+      <c r="D172" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="E172" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E172" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -5922,7 +5913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -5939,7 +5930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -5956,41 +5947,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="4">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
         <v>175</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C176" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="D176" s="4" t="s">
+      <c r="D176" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="E176" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="4">
+      <c r="E176" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
         <v>176</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="C177" s="4" t="s">
+      <c r="C177" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D177" s="4" t="s">
+      <c r="D177" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="E177" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E177" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -6007,7 +5998,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -6024,7 +6015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -6041,7 +6032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -6058,7 +6049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -6075,7 +6066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -6092,7 +6083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -6109,7 +6100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -6126,398 +6117,398 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
         <v>185</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="C186" s="4" t="s">
+      <c r="C186" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D186" s="4" t="s">
+      <c r="D186" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="E186" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="4">
+      <c r="E186" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
         <v>186</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="C187" s="4" t="s">
+      <c r="C187" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D187" s="4" t="s">
+      <c r="D187" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="E187" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4">
+      <c r="E187" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
         <v>187</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="C188" s="4" t="s">
+      <c r="C188" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="D188" s="4" t="s">
+      <c r="D188" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="E188" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4">
+      <c r="E188" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
         <v>188</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B189" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="C189" s="4" t="s">
+      <c r="C189" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E189" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="4">
+      <c r="E189" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
         <v>189</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B190" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="C190" s="4" t="s">
+      <c r="C190" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="D190" s="4" t="s">
+      <c r="D190" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="E190" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4">
+      <c r="E190" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
         <v>190</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B191" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="C191" s="4" t="s">
+      <c r="C191" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="D191" s="4" t="s">
+      <c r="D191" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E191" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="4">
+      <c r="E191" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
         <v>191</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B192" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D192" s="4" t="s">
+      <c r="D192" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E192" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="4">
+      <c r="E192" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
         <v>192</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B193" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="C193" s="4" t="s">
+      <c r="C193" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="D193" s="4" t="s">
+      <c r="D193" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="E193" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="4">
+      <c r="E193" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
         <v>193</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B194" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C194" s="4" t="s">
+      <c r="C194" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="D194" s="4" t="s">
+      <c r="D194" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="E194" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="4">
+      <c r="E194" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
         <v>194</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B195" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="C195" s="4" t="s">
+      <c r="C195" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="D195" s="4" t="s">
+      <c r="D195" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="E195" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4">
+      <c r="E195" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
         <v>195</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B196" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C196" s="4" t="s">
+      <c r="C196" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D196" s="4" t="s">
+      <c r="D196" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="E196" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="4">
+      <c r="E196" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
         <v>196</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B197" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="C197" s="4" t="s">
+      <c r="C197" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="D197" s="4" t="s">
+      <c r="D197" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="E197" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="4">
+      <c r="E197" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
         <v>197</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="B198" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="C198" s="4" t="s">
+      <c r="C198" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="D198" s="4" t="s">
+      <c r="D198" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="E198" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="4">
+      <c r="E198" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
         <v>198</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B199" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="C199" s="4" t="s">
+      <c r="C199" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="D199" s="4" t="s">
+      <c r="D199" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E199" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="4">
+      <c r="E199" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
         <v>199</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B200" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="C200" s="4" t="s">
+      <c r="C200" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="D200" s="4" t="s">
+      <c r="D200" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="E200" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="4">
+      <c r="E200" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
         <v>200</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="B201" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="C201" s="4" t="s">
+      <c r="C201" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="D201" s="4" t="s">
+      <c r="D201" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="E201" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="4">
+      <c r="E201" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
         <v>201</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="B202" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="C202" s="4" t="s">
+      <c r="C202" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="D202" s="4" t="s">
+      <c r="D202" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E202" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="4">
+      <c r="E202" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
         <v>202</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="B203" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="C203" s="4" t="s">
+      <c r="C203" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="D203" s="4" t="s">
+      <c r="D203" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E203" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4">
+      <c r="E203" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
         <v>203</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B204" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="C204" s="4" t="s">
+      <c r="C204" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="D204" s="4" t="s">
+      <c r="D204" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="E204" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="4">
+      <c r="E204" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
         <v>204</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B205" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="C205" s="4" t="s">
+      <c r="C205" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="D205" s="4" t="s">
+      <c r="D205" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="E205" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="4">
+      <c r="E205" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
         <v>205</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B206" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="C206" s="4" t="s">
+      <c r="C206" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="D206" s="4" t="s">
+      <c r="D206" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="E206" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="4">
+      <c r="E206" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
         <v>206</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="B207" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="C207" s="4" t="s">
+      <c r="C207" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="D207" s="4" t="s">
+      <c r="D207" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E207" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="4">
+      <c r="E207" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
         <v>207</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="B208" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C208" s="4" t="s">
+      <c r="C208" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D208" s="4" t="s">
+      <c r="D208" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="E208" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E208" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -6534,7 +6525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -6551,24 +6542,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
         <v>210</v>
       </c>
-      <c r="B211" s="3" t="s">
+      <c r="B211" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="C211" s="3" t="s">
+      <c r="C211" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="D211" s="3" t="s">
+      <c r="D211" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="E211" s="3" t="s">
+      <c r="E211" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -6585,7 +6576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -6602,7 +6593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -6619,7 +6610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -6636,7 +6627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -6653,7 +6644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -6670,7 +6661,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -6687,7 +6678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -6704,41 +6695,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="4">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
         <v>219</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B220" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="C220" s="4" t="s">
+      <c r="C220" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D220" s="4" t="s">
+      <c r="D220" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="E220" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="4">
+      <c r="E220" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
         <v>220</v>
       </c>
-      <c r="B221" s="4" t="s">
+      <c r="B221" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="C221" s="4" t="s">
+      <c r="C221" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D221" s="4" t="s">
+      <c r="D221" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E221" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E221" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -6755,7 +6746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -6772,7 +6763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -6789,7 +6780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -6806,7 +6797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -6823,41 +6814,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="4">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
         <v>226</v>
       </c>
-      <c r="B227" s="4" t="s">
+      <c r="B227" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="C227" s="4" t="s">
+      <c r="C227" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="D227" s="4" t="s">
+      <c r="D227" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="E227" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="4">
+      <c r="E227" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
         <v>227</v>
       </c>
-      <c r="B228" s="4" t="s">
+      <c r="B228" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="C228" s="4" t="s">
+      <c r="C228" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="D228" s="4" t="s">
+      <c r="D228" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="E228" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E228" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -6874,14 +6865,23 @@
         <v>685</v>
       </c>
     </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>229</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C230" s="2"/>
+      <c r="D230" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E229" xr:uid="{2DA76379-63C1-4300-B762-27DAAC682BAD}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Pattern"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E229" xr:uid="{2DA76379-63C1-4300-B762-27DAAC682BAD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected FD length file and Rules control file
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.TestDataGenerator.Functors/FD/Manual/FD Rules Control File.xlsx
+++ b/src/ESFA.DC.ILR.TestDataGenerator.Functors/FD/Manual/FD Rules Control File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAwaghade\OneDrive - Department for Education\Documents\ESFA\FD Rules Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AAwaghade\OneDrive - Department for Education\Documents\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{2E12C40A-DB92-427E-9175-BC7CC62A423E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{6BBCA4B5-33FF-40C2-AF43-E06CBD84461A}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{2E12C40A-DB92-427E-9175-BC7CC62A423E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{25D1C5F5-E44C-41A9-8098-7BECB199B294}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="FD Rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FD Rules'!$A$1:$E$229</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FD Rules'!$A$1:$E$230</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -446,9 +447,6 @@
     <t xml:space="preserve"> The length of the value returned for LearnRefNumber is not between 1 and 12 characters</t>
   </si>
   <si>
-    <t>L49LearnRef</t>
-  </si>
-  <si>
     <t>FD_PrevLearnRefNumber_AL</t>
   </si>
   <si>
@@ -1532,18 +1530,12 @@
     <t xml:space="preserve"> The value returned for ProvSpecDelMonOccur is not 1 character long</t>
   </si>
   <si>
-    <t>L175ProSpOc</t>
-  </si>
-  <si>
     <t>FD_ProvSpecDelMon_AL</t>
   </si>
   <si>
     <t xml:space="preserve"> The length of the value returned for ProvSpecDelMon is not between 1 and 20 characters</t>
   </si>
   <si>
-    <t>L176ProSpDl</t>
-  </si>
-  <si>
     <t>FD_ProviderSpecDeliveryMonitoring_EO</t>
   </si>
   <si>
@@ -1910,15 +1902,9 @@
     <t>FD_DP_LearnRefNumber_AL</t>
   </si>
   <si>
-    <t>L219DP_Lref</t>
-  </si>
-  <si>
     <t>FD_DP_ULN_AL</t>
   </si>
   <si>
-    <t>L220DP_ULN</t>
-  </si>
-  <si>
     <t>FD_DP_ULN_AR</t>
   </si>
   <si>
@@ -1964,18 +1950,12 @@
     <t xml:space="preserve"> The length of the value returned for OutType is not between 1 and 3 characters</t>
   </si>
   <si>
-    <t>L226DP_OutT</t>
-  </si>
-  <si>
     <t>FD_DP_OutCode_AL</t>
   </si>
   <si>
     <t xml:space="preserve"> The length of the value returned for OutCode is not between 1 and 3 characters</t>
   </si>
   <si>
-    <t>L227DP_OutC</t>
-  </si>
-  <si>
     <t>FD_DP_DPOutcome_EO</t>
   </si>
   <si>
@@ -2100,6 +2080,27 @@
   </si>
   <si>
     <t>FD_AgreeId_AP</t>
+  </si>
+  <si>
+    <t>L49LearnRefMoreThan12Chars</t>
+  </si>
+  <si>
+    <t>L227DPOutC</t>
+  </si>
+  <si>
+    <t>L226DPOutT</t>
+  </si>
+  <si>
+    <t>L220DPULN</t>
+  </si>
+  <si>
+    <t>L219DPLref &amp; L219DPLearningRefNumber</t>
+  </si>
+  <si>
+    <t>L176ProSDMon</t>
+  </si>
+  <si>
+    <t>L175ProSDOcc</t>
   </si>
 </sst>
 </file>
@@ -2957,18 +2958,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="80.28515625" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2980,16 +2982,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3023,7 +3025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3040,7 +3042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3057,7 +3059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3108,7 +3110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3125,7 +3127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3136,13 +3138,13 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3159,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3176,7 +3178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3193,7 +3195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3210,7 +3212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3227,7 +3229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3244,7 +3246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3261,7 +3263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3272,13 +3274,13 @@
         <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3289,13 +3291,13 @@
         <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3306,13 +3308,13 @@
         <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3323,13 +3325,13 @@
         <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3357,13 +3359,13 @@
         <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3380,7 +3382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3408,13 +3410,13 @@
         <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3431,7 +3433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3448,7 +3450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3476,13 +3478,13 @@
         <v>84</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3493,13 +3495,13 @@
         <v>86</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3516,7 +3518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3527,13 +3529,13 @@
         <v>91</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3544,13 +3546,13 @@
         <v>93</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3584,7 +3586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3601,7 +3603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3612,13 +3614,13 @@
         <v>104</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3635,7 +3637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3652,7 +3654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3663,13 +3665,13 @@
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3686,7 +3688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3703,7 +3705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3720,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3737,7 +3739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3754,7 +3756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3771,7 +3773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3788,7 +3790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3816,7 +3818,7 @@
         <v>137</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>138</v>
+        <v>683</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>17</v>
@@ -3827,13 +3829,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>17</v>
@@ -3844,13 +3846,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>17</v>
@@ -3861,13 +3863,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>17</v>
@@ -3878,13 +3880,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>17</v>
@@ -3895,13 +3897,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>17</v>
@@ -3912,13 +3914,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>17</v>
@@ -3929,13 +3931,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>17</v>
@@ -3946,13 +3948,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>17</v>
@@ -3963,13 +3965,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>17</v>
@@ -3980,13 +3982,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>17</v>
@@ -3997,13 +3999,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>17</v>
@@ -4014,13 +4016,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>17</v>
@@ -4031,13 +4033,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>17</v>
@@ -4048,13 +4050,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>17</v>
@@ -4065,13 +4067,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>17</v>
@@ -4082,13 +4084,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>17</v>
@@ -4099,13 +4101,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>17</v>
@@ -4116,13 +4118,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>17</v>
@@ -4133,13 +4135,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>17</v>
@@ -4150,13 +4152,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>17</v>
@@ -4167,13 +4169,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>17</v>
@@ -4184,13 +4186,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>17</v>
@@ -4201,13 +4203,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>17</v>
@@ -4218,13 +4220,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>17</v>
@@ -4235,149 +4237,149 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="E75" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="D76" s="2" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>9</v>
@@ -4388,13 +4390,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>17</v>
@@ -4405,47 +4407,47 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="E85" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>9</v>
@@ -4456,13 +4458,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>17</v>
@@ -4473,64 +4475,64 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="E89" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="D90" s="2" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>9</v>
@@ -4541,13 +4543,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>17</v>
@@ -4558,64 +4560,64 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="E94" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="D95" s="2" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>9</v>
@@ -4626,13 +4628,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>17</v>
@@ -4643,64 +4645,64 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="E99" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="D100" s="2" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>9</v>
@@ -4711,13 +4713,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>17</v>
@@ -4728,47 +4730,47 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="E104" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>9</v>
@@ -4779,13 +4781,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>17</v>
@@ -4796,33 +4798,33 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="E108" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="D109" s="2" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4830,13 +4832,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>17</v>
@@ -4847,81 +4849,81 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="E111" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>317</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>319</v>
-      </c>
       <c r="D113" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>9</v>
@@ -4932,13 +4934,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>17</v>
@@ -4949,183 +4951,183 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="E117" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="D118" s="2" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="D119" s="2" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="D123" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="D124" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="D125" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="D126" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="D127" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>359</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>9</v>
@@ -5136,13 +5138,13 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>17</v>
@@ -5153,13 +5155,13 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="D129" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>17</v>
@@ -5170,13 +5172,13 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="D130" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>368</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>17</v>
@@ -5187,13 +5189,13 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="D131" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>17</v>
@@ -5204,13 +5206,13 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>17</v>
@@ -5221,13 +5223,13 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="D133" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>17</v>
@@ -5238,13 +5240,13 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="D134" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>17</v>
@@ -5255,13 +5257,13 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="D135" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>17</v>
@@ -5272,13 +5274,13 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C136" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="D136" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>17</v>
@@ -5289,13 +5291,13 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>17</v>
@@ -5306,13 +5308,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="D138" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>17</v>
@@ -5323,13 +5325,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="D139" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>17</v>
@@ -5340,13 +5342,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="D140" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>17</v>
@@ -5357,13 +5359,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C141" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="D141" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>17</v>
@@ -5374,13 +5376,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="D142" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>17</v>
@@ -5391,13 +5393,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="D143" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>17</v>
@@ -5408,13 +5410,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="D144" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>17</v>
@@ -5425,13 +5427,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="D145" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>17</v>
@@ -5442,13 +5444,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="D146" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>17</v>
@@ -5459,13 +5461,13 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="D147" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>17</v>
@@ -5476,149 +5478,149 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C148" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="D148" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D148" s="2" t="s">
-        <v>422</v>
-      </c>
       <c r="E148" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>424</v>
-      </c>
       <c r="D149" s="2" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="D150" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="D151" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>430</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>432</v>
-      </c>
       <c r="D152" s="2" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>434</v>
-      </c>
       <c r="D153" s="2" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>436</v>
-      </c>
       <c r="D154" s="2" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="D155" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="D156" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>9</v>
@@ -5629,13 +5631,13 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C157" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="D157" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>17</v>
@@ -5646,64 +5648,64 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C158" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="D158" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="D158" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="E158" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C159" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="D159" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="D160" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>454</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="D161" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>9</v>
@@ -5714,13 +5716,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C162" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="D162" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>460</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>17</v>
@@ -5731,13 +5733,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="D163" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>17</v>
@@ -5748,98 +5750,98 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C164" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="D164" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D164" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="E164" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C165" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C165" s="2" t="s">
-        <v>468</v>
-      </c>
       <c r="D165" s="2" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C166" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="D166" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="D167" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="D168" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C169" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="D169" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>480</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>9</v>
@@ -5850,13 +5852,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="D170" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>17</v>
@@ -5867,13 +5869,13 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="D171" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>486</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>17</v>
@@ -5884,64 +5886,64 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="D172" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="D172" s="2" t="s">
-        <v>489</v>
-      </c>
       <c r="E172" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>491</v>
-      </c>
       <c r="D173" s="2" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="D174" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>494</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>497</v>
       </c>
       <c r="E175" s="2" t="s">
         <v>9</v>
@@ -5952,13 +5954,13 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C176" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>499</v>
-      </c>
       <c r="D176" s="2" t="s">
-        <v>500</v>
+        <v>689</v>
       </c>
       <c r="E176" s="2" t="s">
         <v>17</v>
@@ -5969,149 +5971,149 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>503</v>
+        <v>688</v>
       </c>
       <c r="E177" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E179" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E180" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E181" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E183" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E184" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E185" s="2" t="s">
         <v>9</v>
@@ -6122,13 +6124,13 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>17</v>
@@ -6139,13 +6141,13 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E187" s="2" t="s">
         <v>17</v>
@@ -6156,13 +6158,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E188" s="2" t="s">
         <v>17</v>
@@ -6173,13 +6175,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E189" s="2" t="s">
         <v>17</v>
@@ -6190,13 +6192,13 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E190" s="2" t="s">
         <v>17</v>
@@ -6207,13 +6209,13 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E191" s="2" t="s">
         <v>17</v>
@@ -6224,13 +6226,13 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E192" s="2" t="s">
         <v>17</v>
@@ -6241,13 +6243,13 @@
         <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E193" s="2" t="s">
         <v>17</v>
@@ -6258,13 +6260,13 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>17</v>
@@ -6275,13 +6277,13 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E195" s="2" t="s">
         <v>17</v>
@@ -6292,13 +6294,13 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E196" s="2" t="s">
         <v>17</v>
@@ -6309,13 +6311,13 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E197" s="2" t="s">
         <v>17</v>
@@ -6326,13 +6328,13 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E198" s="2" t="s">
         <v>17</v>
@@ -6343,13 +6345,13 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E199" s="2" t="s">
         <v>17</v>
@@ -6360,13 +6362,13 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E200" s="2" t="s">
         <v>17</v>
@@ -6377,13 +6379,13 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E201" s="2" t="s">
         <v>17</v>
@@ -6394,13 +6396,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E202" s="2" t="s">
         <v>17</v>
@@ -6411,13 +6413,13 @@
         <v>202</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E203" s="2" t="s">
         <v>17</v>
@@ -6428,13 +6430,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E204" s="2" t="s">
         <v>17</v>
@@ -6445,13 +6447,13 @@
         <v>204</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E205" s="2" t="s">
         <v>17</v>
@@ -6462,13 +6464,13 @@
         <v>205</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E206" s="2" t="s">
         <v>17</v>
@@ -6479,13 +6481,13 @@
         <v>206</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E207" s="2" t="s">
         <v>17</v>
@@ -6496,200 +6498,200 @@
         <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E208" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E209" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>209</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E210" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>210</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E211" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>211</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E212" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E213" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>213</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E214" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E215" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>215</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="E216" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>217</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>116</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E218" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>119</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E219" s="2" t="s">
         <v>9</v>
@@ -6700,13 +6702,13 @@
         <v>219</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>626</v>
+        <v>687</v>
       </c>
       <c r="E220" s="2" t="s">
         <v>17</v>
@@ -6717,98 +6719,98 @@
         <v>220</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>628</v>
+        <v>686</v>
       </c>
       <c r="E221" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>221</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E222" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E223" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>223</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E224" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="E225" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>225</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E226" s="2" t="s">
         <v>9</v>
@@ -6819,13 +6821,13 @@
         <v>226</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>644</v>
+        <v>685</v>
       </c>
       <c r="E227" s="2" t="s">
         <v>17</v>
@@ -6836,52 +6838,58 @@
         <v>227</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>647</v>
+        <v>684</v>
       </c>
       <c r="E228" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="E229" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>229</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" s="2" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="E230" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E229" xr:uid="{2DA76379-63C1-4300-B762-27DAAC682BAD}"/>
+  <autoFilter ref="A1:E230" xr:uid="{2DA76379-63C1-4300-B762-27DAAC682BAD}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Length"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>